<commit_message>
police bit ko estimate with upvc
</commit_message>
<xml_diff>
--- a/ofc/estimates/kalimasta mandir/kalimasta mandir.xlsx
+++ b/ofc/estimates/kalimasta mandir/kalimasta mandir.xlsx
@@ -2,29 +2,31 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\kalimasta mandir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\kalimasta mandir\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="WCR" sheetId="6" r:id="rId1"/>
     <sheet name="kalimasta mandir final" sheetId="17" r:id="rId2"/>
+    <sheet name="kalimasta mandir final (2)" sheetId="18" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="description_103">[1]Abstract!$B$16</definedName>
     <definedName name="description_124" localSheetId="1">#REF!</definedName>
+    <definedName name="description_124" localSheetId="2">#REF!</definedName>
     <definedName name="description_124">#REF!</definedName>
     <definedName name="description_247">[1]Abstract!$B$22</definedName>
     <definedName name="description_248">[1]Abstract!$B$23</definedName>
@@ -39,10 +41,12 @@
     <definedName name="description_781">[5]Abstract!$B$299</definedName>
     <definedName name="description_783">[1]Abstract!$B$301</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'kalimasta mandir final'!$A$1:$K$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'kalimasta mandir final (2)'!$A$1:$K$63</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'kalimasta mandir final'!$1:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'kalimasta mandir final (2)'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="63">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -234,15 +238,30 @@
   </si>
   <si>
     <t>-stirrups</t>
+  </si>
+  <si>
+    <t>-slab bottom bars</t>
+  </si>
+  <si>
+    <t>-slab top bars along x-axis</t>
+  </si>
+  <si>
+    <t>-slab top bars along y-axis</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>-column</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -412,7 +431,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -422,7 +441,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -442,14 +461,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -458,7 +477,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -483,7 +502,7 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -524,7 +543,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -539,7 +558,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -555,73 +574,73 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1245,106 +1264,106 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-    </row>
-    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="70" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+    </row>
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="65" t="s">
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="65" t="s">
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-    </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="71" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="67" t="e">
+      <c r="C6" s="70" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="68"/>
+      <c r="D6" s="71"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -1352,90 +1371,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="67" t="e">
+      <c r="J6" s="70" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="68"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="71"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="I7" s="75" t="s">
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="I7" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="61" t="e">
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="64" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="I8" s="76" t="s">
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="I8" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="76"/>
-      <c r="K8" s="76"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="77" t="e">
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="68" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="I9" s="76" t="s">
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="I9" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="72" t="s">
+      <c r="J9" s="67"/>
+      <c r="K9" s="67"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="72" t="s">
+      <c r="C11" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="78" t="s">
+      <c r="D11" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78" t="s">
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="72" t="s">
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="73" t="s">
+      <c r="K11" s="63" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="72"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="62"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -1454,10 +1473,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="72"/>
-      <c r="K12" s="73"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="J12" s="62"/>
+      <c r="K12" s="63"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1500,7 +1519,7 @@
       </c>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
       <c r="B14" s="33" t="e">
         <f>#REF!</f>
@@ -1522,7 +1541,7 @@
       <c r="J14" s="28"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="12"/>
@@ -1535,7 +1554,7 @@
       <c r="J15" s="28"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1578,7 +1597,7 @@
       </c>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
       <c r="C17" s="12"/>
@@ -1591,7 +1610,7 @@
       <c r="J17" s="28"/>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>16</v>
@@ -1617,6 +1636,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -1630,13 +1656,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1654,135 +1673,135 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-    </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="64" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-    </row>
-    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="65" t="s">
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+    </row>
+    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-    </row>
-    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="65" t="s">
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+    </row>
+    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-    </row>
-    <row r="5" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="66" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+    </row>
+    <row r="5" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-    </row>
-    <row r="6" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="61" t="s">
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="62" t="s">
+      <c r="H6" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-    </row>
-    <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="79" t="s">
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="80" t="s">
+      <c r="H7" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
-    </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
+    </row>
+    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1817,11 +1836,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>1</v>
       </c>
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="61" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="38"/>
@@ -1834,7 +1853,7 @@
       <c r="J9" s="38"/>
       <c r="K9" s="38"/>
     </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="39" t="s">
         <v>49</v>
@@ -1868,7 +1887,7 @@
       <c r="Q10" s="25"/>
       <c r="R10" s="25"/>
     </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="39" t="s">
         <v>42</v>
@@ -1899,7 +1918,7 @@
       <c r="Q11" s="25"/>
       <c r="R11" s="25"/>
     </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="39" t="s">
         <v>40</v>
@@ -1923,7 +1942,7 @@
       <c r="Q12" s="25"/>
       <c r="R12" s="25"/>
     </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="39"/>
       <c r="C13" s="19"/>
@@ -1942,11 +1961,11 @@
       <c r="Q13" s="25"/>
       <c r="R13" s="25"/>
     </row>
-    <row r="14" spans="1:18" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
         <v>2</v>
       </c>
-      <c r="B14" s="83" t="s">
+      <c r="B14" s="61" t="s">
         <v>50</v>
       </c>
       <c r="C14" s="38"/>
@@ -1959,7 +1978,7 @@
       <c r="J14" s="38"/>
       <c r="K14" s="38"/>
     </row>
-    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="39" t="s">
         <v>49</v>
@@ -1993,7 +2012,7 @@
       <c r="Q15" s="25"/>
       <c r="R15" s="25"/>
     </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="39" t="s">
         <v>42</v>
@@ -2024,7 +2043,7 @@
       <c r="Q16" s="25"/>
       <c r="R16" s="25"/>
     </row>
-    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="39" t="s">
         <v>40</v>
@@ -2048,7 +2067,7 @@
       <c r="Q17" s="25"/>
       <c r="R17" s="25"/>
     </row>
-    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="39"/>
       <c r="C18" s="19"/>
@@ -2067,11 +2086,11 @@
       <c r="Q18" s="25"/>
       <c r="R18" s="25"/>
     </row>
-    <row r="19" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
         <v>3</v>
       </c>
-      <c r="B19" s="83" t="s">
+      <c r="B19" s="61" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="19"/>
@@ -2090,7 +2109,7 @@
       <c r="Q19" s="25"/>
       <c r="R19" s="25"/>
     </row>
-    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
       <c r="B20" s="39" t="s">
         <v>52</v>
@@ -2124,7 +2143,7 @@
       <c r="Q20" s="25"/>
       <c r="R20" s="25"/>
     </row>
-    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="39" t="s">
         <v>53</v>
@@ -2157,7 +2176,7 @@
       <c r="Q21" s="25"/>
       <c r="R21" s="25"/>
     </row>
-    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="39"/>
       <c r="C22" s="19">
@@ -2188,7 +2207,7 @@
       <c r="Q22" s="25"/>
       <c r="R22" s="25"/>
     </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="39" t="s">
         <v>42</v>
@@ -2219,7 +2238,7 @@
       <c r="Q23" s="25"/>
       <c r="R23" s="25"/>
     </row>
-    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="39" t="s">
         <v>40</v>
@@ -2243,7 +2262,7 @@
       <c r="Q24" s="25"/>
       <c r="R24" s="25"/>
     </row>
-    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="39"/>
       <c r="C25" s="19"/>
@@ -2262,11 +2281,11 @@
       <c r="Q25" s="25"/>
       <c r="R25" s="25"/>
     </row>
-    <row r="26" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
         <v>4</v>
       </c>
-      <c r="B26" s="83" t="s">
+      <c r="B26" s="61" t="s">
         <v>54</v>
       </c>
       <c r="C26" s="19"/>
@@ -2285,7 +2304,7 @@
       <c r="Q26" s="25"/>
       <c r="R26" s="25"/>
     </row>
-    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="39" t="str">
         <f>B20</f>
@@ -2319,7 +2338,7 @@
       <c r="Q27" s="25"/>
       <c r="R27" s="25"/>
     </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="39" t="str">
         <f>B21</f>
@@ -2353,7 +2372,7 @@
       <c r="Q28" s="25"/>
       <c r="R28" s="25"/>
     </row>
-    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="39"/>
       <c r="C29" s="19">
@@ -2384,7 +2403,7 @@
       <c r="Q29" s="25"/>
       <c r="R29" s="25"/>
     </row>
-    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="39" t="s">
         <v>42</v>
@@ -2415,7 +2434,7 @@
       <c r="Q30" s="25"/>
       <c r="R30" s="25"/>
     </row>
-    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="39" t="s">
         <v>40</v>
@@ -2439,7 +2458,7 @@
       <c r="Q31" s="25"/>
       <c r="R31" s="25"/>
     </row>
-    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="39"/>
       <c r="C32" s="19"/>
@@ -2458,11 +2477,11 @@
       <c r="Q32" s="25"/>
       <c r="R32" s="25"/>
     </row>
-    <row r="33" spans="1:18" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="18">
         <v>5</v>
       </c>
-      <c r="B33" s="83" t="s">
+      <c r="B33" s="61" t="s">
         <v>55</v>
       </c>
       <c r="C33" s="19" t="s">
@@ -2489,7 +2508,7 @@
       <c r="Q33" s="25"/>
       <c r="R33" s="25"/>
     </row>
-    <row r="34" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="39" t="str">
         <f>B27</f>
@@ -2526,7 +2545,7 @@
       <c r="Q34" s="25"/>
       <c r="R34" s="25"/>
     </row>
-    <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
       <c r="B35" s="39"/>
       <c r="C35" s="19">
@@ -2560,7 +2579,7 @@
       <c r="Q35" s="25"/>
       <c r="R35" s="25"/>
     </row>
-    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="39" t="str">
         <f>B28</f>
@@ -2597,7 +2616,7 @@
       <c r="Q36" s="25"/>
       <c r="R36" s="25"/>
     </row>
-    <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="39"/>
       <c r="C37" s="19">
@@ -2631,7 +2650,7 @@
       <c r="Q37" s="25"/>
       <c r="R37" s="25"/>
     </row>
-    <row r="38" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18"/>
       <c r="B38" s="39" t="s">
         <v>57</v>
@@ -2667,7 +2686,7 @@
       <c r="Q38" s="25"/>
       <c r="R38" s="25"/>
     </row>
-    <row r="39" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
       <c r="B39" s="39"/>
       <c r="C39" s="19">
@@ -2701,7 +2720,7 @@
       <c r="Q39" s="25"/>
       <c r="R39" s="25"/>
     </row>
-    <row r="40" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
       <c r="B40" s="39" t="s">
         <v>42</v>
@@ -2732,7 +2751,7 @@
       <c r="Q40" s="25"/>
       <c r="R40" s="25"/>
     </row>
-    <row r="41" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18"/>
       <c r="B41" s="39" t="s">
         <v>40</v>
@@ -2756,7 +2775,7 @@
       <c r="Q41" s="25"/>
       <c r="R41" s="25"/>
     </row>
-    <row r="42" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
       <c r="B42" s="39"/>
       <c r="C42" s="19"/>
@@ -2775,7 +2794,7 @@
       <c r="Q42" s="25"/>
       <c r="R42" s="25"/>
     </row>
-    <row r="43" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18">
         <v>6</v>
       </c>
@@ -2810,7 +2829,7 @@
       <c r="Q43" s="25"/>
       <c r="R43" s="25"/>
     </row>
-    <row r="44" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="24"/>
       <c r="C44" s="19"/>
@@ -2829,7 +2848,7 @@
       <c r="Q44" s="25"/>
       <c r="R44" s="25"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="42"/>
       <c r="B45" s="44" t="s">
         <v>17</v>
@@ -2847,7 +2866,7 @@
       </c>
       <c r="K45" s="38"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="56"/>
       <c r="B46" s="59"/>
       <c r="C46" s="60"/>
@@ -2860,16 +2879,16 @@
       <c r="J46" s="58"/>
       <c r="K46" s="55"/>
     </row>
-    <row r="47" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="48"/>
       <c r="B47" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C47" s="81">
+      <c r="C47" s="76">
         <f>J45</f>
         <v>345993.93824887183</v>
       </c>
-      <c r="D47" s="81"/>
+      <c r="D47" s="76"/>
       <c r="E47" s="41">
         <v>100</v>
       </c>
@@ -2880,15 +2899,15 @@
       <c r="J47" s="52"/>
       <c r="K47" s="53"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="54"/>
       <c r="B48" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C48" s="82">
+      <c r="C48" s="79">
         <v>300000</v>
       </c>
-      <c r="D48" s="82"/>
+      <c r="D48" s="79"/>
       <c r="E48" s="41"/>
       <c r="F48" s="47"/>
       <c r="G48" s="46"/>
@@ -2897,16 +2916,16 @@
       <c r="J48" s="46"/>
       <c r="K48" s="47"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="54"/>
       <c r="B49" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="82">
+      <c r="C49" s="79">
         <f>C48-C51-C52</f>
         <v>285000</v>
       </c>
-      <c r="D49" s="82"/>
+      <c r="D49" s="79"/>
       <c r="E49" s="41">
         <f>C49/C47*100</f>
         <v>82.371385302999386</v>
@@ -2918,16 +2937,16 @@
       <c r="J49" s="46"/>
       <c r="K49" s="47"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="54"/>
       <c r="B50" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="81">
+      <c r="C50" s="76">
         <f>C47-C49</f>
         <v>60993.938248871826</v>
       </c>
-      <c r="D50" s="81"/>
+      <c r="D50" s="76"/>
       <c r="E50" s="41">
         <f>100-E49</f>
         <v>17.628614697000614</v>
@@ -2939,16 +2958,16 @@
       <c r="J50" s="46"/>
       <c r="K50" s="47"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="54"/>
       <c r="B51" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C51" s="81">
+      <c r="C51" s="76">
         <f>C48*0.03</f>
         <v>9000</v>
       </c>
-      <c r="D51" s="81"/>
+      <c r="D51" s="76"/>
       <c r="E51" s="41">
         <v>3</v>
       </c>
@@ -2959,16 +2978,16 @@
       <c r="J51" s="46"/>
       <c r="K51" s="47"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="54"/>
       <c r="B52" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C52" s="81">
+      <c r="C52" s="76">
         <f>C48*0.02</f>
         <v>6000</v>
       </c>
-      <c r="D52" s="81"/>
+      <c r="D52" s="76"/>
       <c r="E52" s="41">
         <v>2</v>
       </c>
@@ -2979,7 +2998,7 @@
       <c r="J52" s="46"/>
       <c r="K52" s="47"/>
     </row>
-    <row r="53" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="55"/>
       <c r="B53" s="55"/>
       <c r="C53" s="55"/>
@@ -2992,64 +3011,71 @@
       <c r="J53" s="55"/>
       <c r="K53" s="55"/>
     </row>
-    <row r="54" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="101" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="102" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="103" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="104" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="105" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="106" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="107" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="108" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="109" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="A7:F7"/>
@@ -3058,13 +3084,1814 @@
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="C50:D50"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPrepared By:
+Kristal Suwal&amp;CChecked By:
+Er. Milan Phuyal&amp;RApproved By:
+Er. Prakash Singh Saud</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R120"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+    </row>
+    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+    </row>
+    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+    </row>
+    <row r="5" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="80" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="77" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="78" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
+    </row>
+    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="29">
+        <v>1</v>
+      </c>
+      <c r="B9" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="38">
+        <v>0</v>
+      </c>
+      <c r="D10" s="40">
+        <f>12.25/3.281</f>
+        <v>3.7336177994513866</v>
+      </c>
+      <c r="E10" s="40">
+        <f>12.25/3.281</f>
+        <v>3.7336177994513866</v>
+      </c>
+      <c r="F10" s="40">
+        <v>0.15</v>
+      </c>
+      <c r="G10" s="41">
+        <f>PRODUCT(C10:F10)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="21"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+    </row>
+    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="23">
+        <f>SUM(G10:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="23">
+        <v>4473.1499999999996</v>
+      </c>
+      <c r="J11" s="43">
+        <f>G11*I11</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="21"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+    </row>
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="43">
+        <f>0.13*G11*3093.15</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="21"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+    </row>
+    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="21"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+    </row>
+    <row r="14" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="29">
+        <v>2</v>
+      </c>
+      <c r="B14" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="38">
+        <v>0</v>
+      </c>
+      <c r="D15" s="40">
+        <f>12.25/3.281</f>
+        <v>3.7336177994513866</v>
+      </c>
+      <c r="E15" s="40">
+        <f>12.25/3.281</f>
+        <v>3.7336177994513866</v>
+      </c>
+      <c r="F15" s="40">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G15" s="41">
+        <f>PRODUCT(C15:F15)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="21"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+    </row>
+    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="23">
+        <f>SUM(G15:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="23">
+        <v>12568.22</v>
+      </c>
+      <c r="J16" s="43">
+        <f>G16*I16</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="21"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+    </row>
+    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="43">
+        <f>0.13*G16*8523.52</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="21"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+    </row>
+    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="21"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="25"/>
+    </row>
+    <row r="19" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="18">
+        <v>3</v>
+      </c>
+      <c r="B19" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="21"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25"/>
+    </row>
+    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="19">
+        <v>1</v>
+      </c>
+      <c r="D20" s="20">
+        <f>32/3.281</f>
+        <v>9.7531240475464784</v>
+      </c>
+      <c r="E20" s="21">
+        <f>18.75/3.281</f>
+        <v>5.7147211216092648</v>
+      </c>
+      <c r="F20" s="21">
+        <v>0.125</v>
+      </c>
+      <c r="G20" s="41">
+        <f>PRODUCT(C20:F20)</f>
+        <v>6.9670479995236381</v>
+      </c>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="21"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+    </row>
+    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="19">
+        <v>4</v>
+      </c>
+      <c r="D21" s="20">
+        <f>14.5/3.281</f>
+        <v>4.4193843340444987</v>
+      </c>
+      <c r="E21" s="21">
+        <v>0.23</v>
+      </c>
+      <c r="F21" s="21">
+        <v>0.23</v>
+      </c>
+      <c r="G21" s="41">
+        <f t="shared" ref="G21:G23" si="0">PRODUCT(C21:F21)</f>
+        <v>0.93514172508381599</v>
+      </c>
+      <c r="H21" s="22"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="21"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="25"/>
+    </row>
+    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="19">
+        <v>3</v>
+      </c>
+      <c r="D22" s="20">
+        <f>16.75/3.281</f>
+        <v>5.1051508686376099</v>
+      </c>
+      <c r="E22" s="21">
+        <v>0.23</v>
+      </c>
+      <c r="F22" s="21">
+        <v>0.23</v>
+      </c>
+      <c r="G22" s="41">
+        <f t="shared" si="0"/>
+        <v>0.81018744285278876</v>
+      </c>
+      <c r="H22" s="22"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="21"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="25"/>
+    </row>
+    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="19">
+        <v>2</v>
+      </c>
+      <c r="D23" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="E23" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="F23" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="G23" s="41">
+        <f t="shared" si="0"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="H23" s="22"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="21"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="25"/>
+    </row>
+    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="23">
+        <f>SUM(G20:G23)</f>
+        <v>8.7663771674602433</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I24" s="23">
+        <v>13568.9</v>
+      </c>
+      <c r="J24" s="43">
+        <f>G24*I24</f>
+        <v>118950.0951475513</v>
+      </c>
+      <c r="K24" s="21"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="25"/>
+    </row>
+    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="43">
+        <f>0.13*G24*9524.2</f>
+        <v>10854.054824382232</v>
+      </c>
+      <c r="K25" s="21"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+    </row>
+    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="21"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="25"/>
+    </row>
+    <row r="27" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="18">
+        <v>4</v>
+      </c>
+      <c r="B27" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="21"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="25"/>
+    </row>
+    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="39" t="str">
+        <f>B20</f>
+        <v>-slab</v>
+      </c>
+      <c r="C28" s="19">
+        <f>C20</f>
+        <v>1</v>
+      </c>
+      <c r="D28" s="20">
+        <f>D20</f>
+        <v>9.7531240475464784</v>
+      </c>
+      <c r="E28" s="21">
+        <f>E20</f>
+        <v>5.7147211216092648</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="41">
+        <f>PRODUCT(C28:F28)</f>
+        <v>55.736383996189105</v>
+      </c>
+      <c r="H28" s="22"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="21"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="25"/>
+    </row>
+    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="39" t="str">
+        <f>B21</f>
+        <v>-beam</v>
+      </c>
+      <c r="C29" s="19">
+        <f>C21</f>
+        <v>4</v>
+      </c>
+      <c r="D29" s="20">
+        <f>D21</f>
+        <v>4.4193843340444987</v>
+      </c>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21">
+        <f>F21*2</f>
+        <v>0.46</v>
+      </c>
+      <c r="G29" s="41">
+        <f t="shared" ref="G29:G31" si="1">PRODUCT(C29:F29)</f>
+        <v>8.131667174641878</v>
+      </c>
+      <c r="H29" s="22"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="21"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="25"/>
+      <c r="R29" s="25"/>
+    </row>
+    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="19">
+        <f>C22</f>
+        <v>3</v>
+      </c>
+      <c r="D30" s="20">
+        <f>D22</f>
+        <v>5.1051508686376099</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21">
+        <f>F22*2</f>
+        <v>0.46</v>
+      </c>
+      <c r="G30" s="41">
+        <f t="shared" si="1"/>
+        <v>7.0451081987199018</v>
+      </c>
+      <c r="H30" s="22"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="21"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="25"/>
+      <c r="R30" s="25"/>
+    </row>
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="19">
+        <f>C23</f>
+        <v>2</v>
+      </c>
+      <c r="D31" s="20">
+        <f>D23*4</f>
+        <v>1.2</v>
+      </c>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21">
+        <f>F23</f>
+        <v>0.3</v>
+      </c>
+      <c r="G31" s="41">
+        <f t="shared" si="1"/>
+        <v>0.72</v>
+      </c>
+      <c r="H31" s="22"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="21"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="25"/>
+      <c r="R31" s="25"/>
+    </row>
+    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
+      <c r="B32" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="23">
+        <f>SUM(G28:G31)</f>
+        <v>71.633159369550881</v>
+      </c>
+      <c r="H32" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I32" s="23">
+        <v>915.42</v>
+      </c>
+      <c r="J32" s="43">
+        <f>G32*I32</f>
+        <v>65574.426750074272</v>
+      </c>
+      <c r="K32" s="21"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="25"/>
+      <c r="R32" s="25"/>
+    </row>
+    <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="43">
+        <f>0.13*G32*46827.87/100</f>
+        <v>4360.7567570405945</v>
+      </c>
+      <c r="K33" s="21"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="25"/>
+      <c r="R33" s="25"/>
+    </row>
+    <row r="34" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="21"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="25"/>
+      <c r="R34" s="25"/>
+    </row>
+    <row r="35" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
+        <v>5</v>
+      </c>
+      <c r="B35" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G35" s="23"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="21"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="25"/>
+      <c r="R35" s="25"/>
+    </row>
+    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="19">
+        <v>34</v>
+      </c>
+      <c r="D36" s="20">
+        <f>31.667/3.281</f>
+        <v>9.6516306004266994</v>
+      </c>
+      <c r="E36" s="21">
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F36" s="41">
+        <f>PRODUCT(C36:E36)</f>
+        <v>129.64165547239813</v>
+      </c>
+      <c r="G36" s="41">
+        <f>F36/1000</f>
+        <v>0.12964165547239812</v>
+      </c>
+      <c r="H36" s="22"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="21"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="25"/>
+      <c r="R36" s="25"/>
+    </row>
+    <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="19">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="D37" s="20">
+        <f>18.42/3.281</f>
+        <v>5.6141420298689431</v>
+      </c>
+      <c r="E37" s="21">
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F37" s="41">
+        <f>PRODUCT(C37:E37)</f>
+        <v>133.07595922652308</v>
+      </c>
+      <c r="G37" s="41">
+        <f>F37/1000</f>
+        <v>0.13307595922652307</v>
+      </c>
+      <c r="H37" s="22"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="43"/>
+      <c r="K37" s="21"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="25"/>
+      <c r="R37" s="25"/>
+    </row>
+    <row r="38" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="19">
+        <f>9*2</f>
+        <v>18</v>
+      </c>
+      <c r="D38" s="20">
+        <f>6.75/3.281</f>
+        <v>2.0572996037793354</v>
+      </c>
+      <c r="E38" s="21">
+        <f t="shared" ref="E38:E42" si="2">8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F38" s="41">
+        <f t="shared" ref="F38:F42" si="3">PRODUCT(C38:E38)</f>
+        <v>14.629686071319718</v>
+      </c>
+      <c r="G38" s="41">
+        <f t="shared" ref="G38:G42" si="4">F38/1000</f>
+        <v>1.4629686071319717E-2</v>
+      </c>
+      <c r="H38" s="22"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="43"/>
+      <c r="K38" s="21"/>
+      <c r="M38" s="1">
+        <f>12.75*0.3</f>
+        <v>3.8249999999999997</v>
+      </c>
+      <c r="N38" s="1">
+        <f>13*0.3</f>
+        <v>3.9</v>
+      </c>
+      <c r="O38" s="1">
+        <f>13/3.281</f>
+        <v>3.9622066443157573</v>
+      </c>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="25"/>
+      <c r="R38" s="25"/>
+    </row>
+    <row r="39" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="18"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="19">
+        <f>9</f>
+        <v>9</v>
+      </c>
+      <c r="D39" s="20">
+        <f>8.583/3.281</f>
+        <v>2.6159707406278572</v>
+      </c>
+      <c r="E39" s="21">
+        <f t="shared" si="2"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F39" s="41">
+        <f t="shared" si="3"/>
+        <v>9.3012293000101582</v>
+      </c>
+      <c r="G39" s="41">
+        <f t="shared" si="4"/>
+        <v>9.3012293000101585E-3</v>
+      </c>
+      <c r="H39" s="22"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="43"/>
+      <c r="K39" s="21"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1">
+        <f>12.75/3.281</f>
+        <v>3.8860103626943006</v>
+      </c>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="25"/>
+      <c r="R39" s="25"/>
+    </row>
+    <row r="40" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="18"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="19">
+        <f>13+12</f>
+        <v>25</v>
+      </c>
+      <c r="D40" s="20">
+        <f>31.667/3.281</f>
+        <v>9.6516306004266994</v>
+      </c>
+      <c r="E40" s="21">
+        <f t="shared" si="2"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F40" s="41">
+        <f t="shared" si="3"/>
+        <v>95.32474667088097</v>
+      </c>
+      <c r="G40" s="41">
+        <f t="shared" si="4"/>
+        <v>9.5324746670880964E-2</v>
+      </c>
+      <c r="H40" s="22"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="21"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="25"/>
+      <c r="R40" s="25"/>
+    </row>
+    <row r="41" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="19">
+        <f>10*4</f>
+        <v>40</v>
+      </c>
+      <c r="D41" s="20">
+        <f>7.083/3.281</f>
+        <v>2.1587930508991162</v>
+      </c>
+      <c r="E41" s="21">
+        <f t="shared" si="2"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F41" s="41">
+        <f t="shared" si="3"/>
+        <v>34.114260557418135</v>
+      </c>
+      <c r="G41" s="41">
+        <f t="shared" si="4"/>
+        <v>3.4114260557418133E-2</v>
+      </c>
+      <c r="H41" s="22"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="21"/>
+      <c r="M41" s="1">
+        <f>12.75*0.3</f>
+        <v>3.8249999999999997</v>
+      </c>
+      <c r="N41" s="1">
+        <f>13*0.3</f>
+        <v>3.9</v>
+      </c>
+      <c r="O41" s="1">
+        <f>13/3.281</f>
+        <v>3.9622066443157573</v>
+      </c>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="25"/>
+      <c r="R41" s="25"/>
+    </row>
+    <row r="42" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="19">
+        <f>10*4</f>
+        <v>40</v>
+      </c>
+      <c r="D42" s="20">
+        <f>18.42/3.281</f>
+        <v>5.6141420298689431</v>
+      </c>
+      <c r="E42" s="21">
+        <f t="shared" si="2"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F42" s="41">
+        <f t="shared" si="3"/>
+        <v>88.717306151015393</v>
+      </c>
+      <c r="G42" s="41">
+        <f t="shared" si="4"/>
+        <v>8.871730615101539E-2</v>
+      </c>
+      <c r="H42" s="22"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="21"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="25"/>
+      <c r="R42" s="25"/>
+    </row>
+    <row r="43" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="41"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="43"/>
+      <c r="K43" s="21"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="25"/>
+      <c r="R43" s="25"/>
+    </row>
+    <row r="44" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="39" t="str">
+        <f>B29</f>
+        <v>-beam</v>
+      </c>
+      <c r="C44" s="19">
+        <f>2*5</f>
+        <v>10</v>
+      </c>
+      <c r="D44" s="20">
+        <f>D20</f>
+        <v>9.7531240475464784</v>
+      </c>
+      <c r="E44" s="21">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F44" s="41">
+        <f t="shared" ref="F44:F47" si="5">PRODUCT(C44:E44)</f>
+        <v>86.69443597819091</v>
+      </c>
+      <c r="G44" s="41">
+        <f t="shared" ref="G44:G47" si="6">F44/1000</f>
+        <v>8.6694435978190904E-2</v>
+      </c>
+      <c r="H44" s="22"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="43"/>
+      <c r="K44" s="21"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="25"/>
+      <c r="R44" s="25"/>
+    </row>
+    <row r="45" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="19">
+        <f>3*5</f>
+        <v>15</v>
+      </c>
+      <c r="D45" s="20">
+        <f>E20</f>
+        <v>5.7147211216092648</v>
+      </c>
+      <c r="E45" s="21">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F45" s="41">
+        <f t="shared" si="5"/>
+        <v>76.196281621456862</v>
+      </c>
+      <c r="G45" s="41">
+        <f t="shared" si="6"/>
+        <v>7.6196281621456863E-2</v>
+      </c>
+      <c r="H45" s="22"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="21"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="25"/>
+      <c r="R45" s="25"/>
+    </row>
+    <row r="46" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="19">
+        <f>37*4</f>
+        <v>148</v>
+      </c>
+      <c r="D46" s="20">
+        <f>(0.3*2+(0.583/3.281)*2+0.075*2)</f>
+        <v>1.1053794574824747</v>
+      </c>
+      <c r="E46" s="21">
+        <f t="shared" ref="E46:E50" si="7">8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F46" s="41">
+        <f t="shared" si="5"/>
+        <v>64.630581612802473</v>
+      </c>
+      <c r="G46" s="41">
+        <f t="shared" si="6"/>
+        <v>6.4630581612802468E-2</v>
+      </c>
+      <c r="H46" s="22"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="43"/>
+      <c r="K46" s="21"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="25"/>
+      <c r="R46" s="25"/>
+    </row>
+    <row r="47" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="19">
+        <f>(29+7+7)*3</f>
+        <v>129</v>
+      </c>
+      <c r="D47" s="20">
+        <f>(0.3*2+(0.583/3.281)*2+0.075*2)</f>
+        <v>1.1053794574824747</v>
+      </c>
+      <c r="E47" s="21">
+        <f t="shared" si="7"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F47" s="41">
+        <f t="shared" si="5"/>
+        <v>56.333412351699451</v>
+      </c>
+      <c r="G47" s="41">
+        <f t="shared" si="6"/>
+        <v>5.6333412351699454E-2</v>
+      </c>
+      <c r="H47" s="22"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="21"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="25"/>
+      <c r="R47" s="25"/>
+    </row>
+    <row r="48" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="18"/>
+      <c r="B48" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="19">
+        <f>6*8</f>
+        <v>48</v>
+      </c>
+      <c r="D48" s="20">
+        <f>12.5/3.281</f>
+        <v>3.8098140810728434</v>
+      </c>
+      <c r="E48" s="21">
+        <f t="shared" ref="E48" si="8">12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F48" s="41">
+        <f t="shared" ref="F48:F50" si="9">PRODUCT(C48:E48)</f>
+        <v>162.55206745910797</v>
+      </c>
+      <c r="G48" s="41">
+        <f t="shared" ref="G48:G50" si="10">F48/1000</f>
+        <v>0.16255206745910797</v>
+      </c>
+      <c r="H48" s="22"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="21"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="25"/>
+      <c r="R48" s="25"/>
+    </row>
+    <row r="49" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
+      <c r="B49" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="19">
+        <f>(8.917/3.281)/0.125</f>
+        <v>21.742151782992988</v>
+      </c>
+      <c r="D49" s="20">
+        <f>(0.23*4+0.075*2)</f>
+        <v>1.07</v>
+      </c>
+      <c r="E49" s="21">
+        <f t="shared" si="7"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F49" s="41">
+        <f t="shared" si="9"/>
+        <v>9.1907565067861707</v>
+      </c>
+      <c r="G49" s="41">
+        <f t="shared" si="10"/>
+        <v>9.1907565067861699E-3</v>
+      </c>
+      <c r="H49" s="22"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="43"/>
+      <c r="K49" s="21"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="25"/>
+      <c r="R49" s="25"/>
+    </row>
+    <row r="50" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="19">
+        <f>(8.917/3.281)/0.125</f>
+        <v>21.742151782992988</v>
+      </c>
+      <c r="D50" s="20">
+        <f>(0.23*4+0.075*2)</f>
+        <v>1.07</v>
+      </c>
+      <c r="E50" s="21">
+        <f t="shared" si="7"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F50" s="41">
+        <f t="shared" si="9"/>
+        <v>9.1907565067861707</v>
+      </c>
+      <c r="G50" s="41">
+        <f t="shared" si="10"/>
+        <v>9.1907565067861699E-3</v>
+      </c>
+      <c r="H50" s="22"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="43"/>
+      <c r="K50" s="21"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="25"/>
+      <c r="R50" s="25"/>
+    </row>
+    <row r="51" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="19"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="23">
+        <f>SUM(G36:G50)</f>
+        <v>0.96959313548639547</v>
+      </c>
+      <c r="H51" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="I51" s="23">
+        <v>131940</v>
+      </c>
+      <c r="J51" s="43">
+        <f>G51*I51</f>
+        <v>127928.11829607502</v>
+      </c>
+      <c r="K51" s="21"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="25"/>
+      <c r="R51" s="25"/>
+    </row>
+    <row r="52" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
+      <c r="B52" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" s="19"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="23"/>
+      <c r="J52" s="43">
+        <f>0.13*G51*106200</f>
+        <v>13386.202828525178</v>
+      </c>
+      <c r="K52" s="21"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="25"/>
+      <c r="R52" s="25"/>
+    </row>
+    <row r="53" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="18"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="23"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="21"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="25"/>
+      <c r="R53" s="25"/>
+    </row>
+    <row r="54" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="18">
+        <v>6</v>
+      </c>
+      <c r="B54" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54" s="19">
+        <v>1</v>
+      </c>
+      <c r="D54" s="20"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="34">
+        <f t="shared" ref="G54" si="11">PRODUCT(C54:F54)</f>
+        <v>1</v>
+      </c>
+      <c r="H54" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I54" s="23">
+        <v>500</v>
+      </c>
+      <c r="J54" s="34">
+        <f>G54*I54</f>
+        <v>500</v>
+      </c>
+      <c r="K54" s="21"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="25"/>
+      <c r="R54" s="25"/>
+    </row>
+    <row r="55" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="18"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="23"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="23"/>
+      <c r="J55" s="43"/>
+      <c r="K55" s="21"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="25"/>
+      <c r="R55" s="25"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56" s="42"/>
+      <c r="B56" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="45"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="43"/>
+      <c r="J56" s="43">
+        <f>SUM(J10:J54)</f>
+        <v>341553.65460364858</v>
+      </c>
+      <c r="K56" s="38"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" s="56"/>
+      <c r="B57" s="59"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="57"/>
+      <c r="E57" s="57"/>
+      <c r="F57" s="57"/>
+      <c r="G57" s="58"/>
+      <c r="H57" s="58"/>
+      <c r="I57" s="58"/>
+      <c r="J57" s="58"/>
+      <c r="K57" s="55"/>
+    </row>
+    <row r="58" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="48"/>
+      <c r="B58" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58" s="76">
+        <f>J56</f>
+        <v>341553.65460364858</v>
+      </c>
+      <c r="D58" s="76"/>
+      <c r="E58" s="41">
+        <v>100</v>
+      </c>
+      <c r="F58" s="49"/>
+      <c r="G58" s="50"/>
+      <c r="H58" s="49"/>
+      <c r="I58" s="51"/>
+      <c r="J58" s="52"/>
+      <c r="K58" s="53"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A59" s="54"/>
+      <c r="B59" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="79">
+        <v>300000</v>
+      </c>
+      <c r="D59" s="79"/>
+      <c r="E59" s="41"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="46"/>
+      <c r="H59" s="46"/>
+      <c r="I59" s="46"/>
+      <c r="J59" s="46"/>
+      <c r="K59" s="47"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A60" s="54"/>
+      <c r="B60" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" s="79">
+        <f>C59-C62-C63</f>
+        <v>285000</v>
+      </c>
+      <c r="D60" s="79"/>
+      <c r="E60" s="41">
+        <f>C60/C58*100</f>
+        <v>83.442234084927151</v>
+      </c>
+      <c r="F60" s="47"/>
+      <c r="G60" s="46"/>
+      <c r="H60" s="46"/>
+      <c r="I60" s="46"/>
+      <c r="J60" s="46"/>
+      <c r="K60" s="47"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" s="54"/>
+      <c r="B61" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="76">
+        <f>C58-C60</f>
+        <v>56553.654603648582</v>
+      </c>
+      <c r="D61" s="76"/>
+      <c r="E61" s="41">
+        <f>100-E60</f>
+        <v>16.557765915072849</v>
+      </c>
+      <c r="F61" s="47"/>
+      <c r="G61" s="46"/>
+      <c r="H61" s="46"/>
+      <c r="I61" s="46"/>
+      <c r="J61" s="46"/>
+      <c r="K61" s="47"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62" s="54"/>
+      <c r="B62" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C62" s="76">
+        <f>C59*0.03</f>
+        <v>9000</v>
+      </c>
+      <c r="D62" s="76"/>
+      <c r="E62" s="41">
+        <v>3</v>
+      </c>
+      <c r="F62" s="47"/>
+      <c r="G62" s="46"/>
+      <c r="H62" s="46"/>
+      <c r="I62" s="46"/>
+      <c r="J62" s="46"/>
+      <c r="K62" s="47"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A63" s="54"/>
+      <c r="B63" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C63" s="76">
+        <f>C59*0.02</f>
+        <v>6000</v>
+      </c>
+      <c r="D63" s="76"/>
+      <c r="E63" s="41">
+        <v>2</v>
+      </c>
+      <c r="F63" s="47"/>
+      <c r="G63" s="46"/>
+      <c r="H63" s="46"/>
+      <c r="I63" s="46"/>
+      <c r="J63" s="46"/>
+      <c r="K63" s="47"/>
+    </row>
+    <row r="64" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="55"/>
+      <c r="B64" s="55"/>
+      <c r="C64" s="55"/>
+      <c r="D64" s="55"/>
+      <c r="E64" s="55"/>
+      <c r="F64" s="55"/>
+      <c r="G64" s="55"/>
+      <c r="H64" s="55"/>
+      <c r="I64" s="55"/>
+      <c r="J64" s="55"/>
+      <c r="K64" s="55"/>
+    </row>
+    <row r="65" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>